<commit_message>
Changes in QUESTIONS table and data
</commit_message>
<xml_diff>
--- a/docs/Test1_Questions_table.xlsx
+++ b/docs/Test1_Questions_table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="17360" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Questions" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
   <si>
     <t>QUESTIONS</t>
   </si>
@@ -386,6 +386,9 @@
   </si>
   <si>
     <t>Cuando nos sentimos amargados, "victimas del destino" y sin darnos cuenta culpamos a nuestro entorno de todo lo que nos pasa. La energía de la flor de sauce nos ayuda a asumir la responsabilidad sobre nuestra propia vida. A ser positivos, constructivos y optimistas, dejando que afloren a nuestra mente pensamientos positivos</t>
+  </si>
+  <si>
+    <t>I_QSTN</t>
   </si>
 </sst>
 </file>
@@ -441,8 +444,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -452,11 +457,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -786,10 +793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -797,12 +804,12 @@
     <col min="1" max="1" width="162.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -810,13 +817,16 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -824,13 +834,16 @@
         <v>1</v>
       </c>
       <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
         <v>20</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -838,13 +851,16 @@
         <v>1</v>
       </c>
       <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
         <v>5</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -852,13 +868,16 @@
         <v>1</v>
       </c>
       <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
         <v>7</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -866,13 +885,16 @@
         <v>1</v>
       </c>
       <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
         <v>23</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -880,13 +902,16 @@
         <v>1</v>
       </c>
       <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
         <v>35</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -894,13 +919,16 @@
         <v>1</v>
       </c>
       <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8">
         <v>18</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -908,13 +936,16 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -922,13 +953,16 @@
         <v>1</v>
       </c>
       <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10">
         <v>15</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -936,13 +970,16 @@
         <v>1</v>
       </c>
       <c r="C11">
+        <v>9</v>
+      </c>
+      <c r="D11">
         <v>11</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -950,13 +987,16 @@
         <v>1</v>
       </c>
       <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12">
         <v>19</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -964,13 +1004,16 @@
         <v>1</v>
       </c>
       <c r="C13">
+        <v>11</v>
+      </c>
+      <c r="D13">
         <v>29</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -978,13 +1021,16 @@
         <v>1</v>
       </c>
       <c r="C14">
+        <v>12</v>
+      </c>
+      <c r="D14">
         <v>8</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -992,13 +1038,16 @@
         <v>1</v>
       </c>
       <c r="C15">
+        <v>13</v>
+      </c>
+      <c r="D15">
         <v>25</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -1006,13 +1055,16 @@
         <v>1</v>
       </c>
       <c r="C16">
+        <v>14</v>
+      </c>
+      <c r="D16">
         <v>2</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -1020,13 +1072,16 @@
         <v>1</v>
       </c>
       <c r="C17">
+        <v>15</v>
+      </c>
+      <c r="D17">
         <v>13</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
@@ -1034,13 +1089,16 @@
         <v>1</v>
       </c>
       <c r="C18">
+        <v>16</v>
+      </c>
+      <c r="D18">
         <v>36</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
@@ -1048,13 +1106,16 @@
         <v>1</v>
       </c>
       <c r="C19">
+        <v>17</v>
+      </c>
+      <c r="D19">
         <v>14</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
@@ -1062,13 +1123,16 @@
         <v>1</v>
       </c>
       <c r="C20">
+        <v>18</v>
+      </c>
+      <c r="D20">
         <v>24</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -1076,13 +1140,16 @@
         <v>1</v>
       </c>
       <c r="C21">
+        <v>19</v>
+      </c>
+      <c r="D21">
         <v>30</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
@@ -1090,13 +1157,16 @@
         <v>1</v>
       </c>
       <c r="C22">
+        <v>20</v>
+      </c>
+      <c r="D22">
         <v>27</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -1104,13 +1174,16 @@
         <v>1</v>
       </c>
       <c r="C23">
+        <v>21</v>
+      </c>
+      <c r="D23">
         <v>32</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
@@ -1118,13 +1191,16 @@
         <v>1</v>
       </c>
       <c r="C24">
+        <v>22</v>
+      </c>
+      <c r="D24">
         <v>10</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
@@ -1132,13 +1208,16 @@
         <v>1</v>
       </c>
       <c r="C25">
+        <v>23</v>
+      </c>
+      <c r="D25">
         <v>22</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
         <v>28</v>
       </c>
@@ -1146,13 +1225,16 @@
         <v>1</v>
       </c>
       <c r="C26">
+        <v>24</v>
+      </c>
+      <c r="D26">
         <v>31</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
@@ -1160,13 +1242,16 @@
         <v>1</v>
       </c>
       <c r="C27">
+        <v>25</v>
+      </c>
+      <c r="D27">
         <v>26</v>
       </c>
-      <c r="D27">
+      <c r="E27">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:5">
       <c r="A28" s="1" t="s">
         <v>30</v>
       </c>
@@ -1174,13 +1259,16 @@
         <v>1</v>
       </c>
       <c r="C28">
+        <v>26</v>
+      </c>
+      <c r="D28">
         <v>6</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
         <v>31</v>
       </c>
@@ -1188,13 +1276,16 @@
         <v>1</v>
       </c>
       <c r="C29">
+        <v>27</v>
+      </c>
+      <c r="D29">
         <v>12</v>
       </c>
-      <c r="D29">
+      <c r="E29">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:5">
       <c r="A30" s="1" t="s">
         <v>32</v>
       </c>
@@ -1202,13 +1293,16 @@
         <v>1</v>
       </c>
       <c r="C30">
+        <v>28</v>
+      </c>
+      <c r="D30">
         <v>16</v>
       </c>
-      <c r="D30">
+      <c r="E30">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:5">
       <c r="A31" s="1" t="s">
         <v>33</v>
       </c>
@@ -1216,13 +1310,16 @@
         <v>1</v>
       </c>
       <c r="C31">
+        <v>29</v>
+      </c>
+      <c r="D31">
         <v>37</v>
       </c>
-      <c r="D31">
+      <c r="E31">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:5">
       <c r="A32" s="1" t="s">
         <v>34</v>
       </c>
@@ -1230,13 +1327,16 @@
         <v>1</v>
       </c>
       <c r="C32">
+        <v>30</v>
+      </c>
+      <c r="D32">
         <v>33</v>
       </c>
-      <c r="D32">
+      <c r="E32">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:5">
       <c r="A33" s="1" t="s">
         <v>35</v>
       </c>
@@ -1244,13 +1344,16 @@
         <v>1</v>
       </c>
       <c r="C33">
+        <v>31</v>
+      </c>
+      <c r="D33">
         <v>3</v>
       </c>
-      <c r="D33">
+      <c r="E33">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:5">
       <c r="A34" s="1" t="s">
         <v>36</v>
       </c>
@@ -1258,13 +1361,16 @@
         <v>1</v>
       </c>
       <c r="C34">
+        <v>32</v>
+      </c>
+      <c r="D34">
         <v>21</v>
       </c>
-      <c r="D34">
+      <c r="E34">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:5">
       <c r="A35" s="1" t="s">
         <v>37</v>
       </c>
@@ -1272,13 +1378,16 @@
         <v>1</v>
       </c>
       <c r="C35">
+        <v>33</v>
+      </c>
+      <c r="D35">
         <v>17</v>
       </c>
-      <c r="D35">
+      <c r="E35">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:5">
       <c r="A36" s="1" t="s">
         <v>38</v>
       </c>
@@ -1286,13 +1395,16 @@
         <v>1</v>
       </c>
       <c r="C36">
+        <v>34</v>
+      </c>
+      <c r="D36">
         <v>38</v>
       </c>
-      <c r="D36">
+      <c r="E36">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:5">
       <c r="A37" s="1" t="s">
         <v>39</v>
       </c>
@@ -1300,13 +1412,16 @@
         <v>1</v>
       </c>
       <c r="C37">
+        <v>35</v>
+      </c>
+      <c r="D37">
         <v>9</v>
       </c>
-      <c r="D37">
+      <c r="E37">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:5">
       <c r="A38" s="1" t="s">
         <v>40</v>
       </c>
@@ -1314,13 +1429,16 @@
         <v>1</v>
       </c>
       <c r="C38">
+        <v>36</v>
+      </c>
+      <c r="D38">
         <v>28</v>
       </c>
-      <c r="D38">
+      <c r="E38">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:5">
       <c r="A39" s="1" t="s">
         <v>41</v>
       </c>
@@ -1328,13 +1446,16 @@
         <v>1</v>
       </c>
       <c r="C39">
+        <v>37</v>
+      </c>
+      <c r="D39">
         <v>34</v>
       </c>
-      <c r="D39">
+      <c r="E39">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:5">
       <c r="A40" s="1" t="s">
         <v>42</v>
       </c>
@@ -1342,14 +1463,18 @@
         <v>1</v>
       </c>
       <c r="C40">
+        <v>38</v>
+      </c>
+      <c r="D40">
         <v>4</v>
       </c>
-      <c r="D40">
+      <c r="E40">
         <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1362,7 +1487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -1691,7 +1816,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>